<commit_message>
added few more stuff
</commit_message>
<xml_diff>
--- a/Rewards.xlsx
+++ b/Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmieren\Python\WoodygameBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C29ECE-429B-45CE-9F58-05415262733C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB2E6D7-35BB-405D-A255-81929FF269DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>freeSpace</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>Runden:</t>
+  </si>
+  <si>
+    <t>BlocksFitting</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,9 +408,10 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -414,11 +421,20 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -428,52 +444,82 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="E2:E9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Made all to a norm
</commit_message>
<xml_diff>
--- a/Rewards.xlsx
+++ b/Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmieren\Python\WoodygameBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB2E6D7-35BB-405D-A255-81929FF269DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454C21F0-E46E-435A-95A7-17ECDAD8DA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>freeSpace</t>
   </si>
@@ -39,10 +39,25 @@
     <t>Avg</t>
   </si>
   <si>
-    <t>Runden:</t>
-  </si>
-  <si>
     <t>BlocksFitting</t>
+  </si>
+  <si>
+    <t>Runden</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Silas</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -84,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,16 +122,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -397,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,115 +442,203 @@
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>655</v>
+      </c>
+      <c r="F2" s="4">
         <v>500</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>600</v>
+      </c>
+      <c r="F3" s="5">
+        <v>500</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>666</v>
+      </c>
+      <c r="F4" s="4">
+        <v>500</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>608</v>
+      </c>
+      <c r="F5" s="5">
+        <v>320</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>10</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E9">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>